<commit_message>
ä zu ae in Fälle table "RKI"
</commit_message>
<xml_diff>
--- a/extData/DE_InfectionCases.xlsx
+++ b/extData/DE_InfectionCases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96714FEF-C082-4159-A232-AD0E8B9B13DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCF49EA-0F59-4DD3-A4CE-91304B528642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="708" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="708" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tageswerte berechnet" sheetId="9" r:id="rId1"/>
@@ -66,12 +66,6 @@
     <t/>
   </si>
   <si>
-    <t>Anzahl COVID-19-Fälle</t>
-  </si>
-  <si>
-    <t>Differenz Vortag Fälle</t>
-  </si>
-  <si>
     <t>Differenz Vortag Todesfälle</t>
   </si>
   <si>
@@ -1606,6 +1600,12 @@
   </si>
   <si>
     <t>LK Schleswig-Flensburg</t>
+  </si>
+  <si>
+    <t>Anzahl COVID-19-Faelle</t>
+  </si>
+  <si>
+    <t>Differenz Vortag Faelle</t>
   </si>
 </sst>
 </file>
@@ -2193,23 +2193,23 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>14829</v>
@@ -2220,7 +2220,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>22100</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>7334</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1924</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>1012</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>1873</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>10708</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>726</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>6770</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>29879</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>5358</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>1225</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>6902</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>1424</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>1394</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>2127</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="22" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
         <f>SUM(B6:B21)</f>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31">
         <v>879564</v>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="35" spans="1:1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
@@ -2451,9 +2451,9 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A2:S510"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I277" sqref="I277"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2467,7 +2467,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
@@ -2475,22 +2475,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>516</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>517</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -7074,7 +7074,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A177" s="32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B177" s="25">
         <v>223453</v>
@@ -7321,7 +7321,7 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A186" s="32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B186" s="27">
         <v>234853</v>
@@ -7528,7 +7528,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A193" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B193" s="25">
         <v>243599</v>
@@ -7718,7 +7718,7 @@
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A200" s="33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B200" s="27">
         <v>252298</v>
@@ -7748,7 +7748,7 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A201" s="33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B201" s="27">
         <v>253474</v>
@@ -7778,7 +7778,7 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A202" s="33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B202" s="27">
         <v>255366</v>
@@ -7808,7 +7808,7 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A203" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B203" s="27">
         <v>256850</v>
@@ -7838,7 +7838,7 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A204" s="33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B204" s="25">
         <v>258480</v>
@@ -7868,7 +7868,7 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A205" s="33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B205" s="25">
         <v>259428</v>
@@ -7898,7 +7898,7 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A206" s="33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B206" s="25">
         <v>260355</v>
@@ -8063,7 +8063,7 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A212" s="33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B212" s="25">
         <v>271415</v>
@@ -8090,7 +8090,7 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A213" s="33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B213" s="25">
         <v>272337</v>
@@ -8117,7 +8117,7 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A214" s="33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B214" s="25">
         <v>274158</v>
@@ -8144,7 +8144,7 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A215" s="33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B215" s="25">
         <v>275927</v>
@@ -8261,7 +8261,7 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A219" s="33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B219" s="25">
         <v>284140</v>
@@ -8288,7 +8288,7 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A220" s="33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B220" s="25">
         <v>285332</v>
@@ -8315,7 +8315,7 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A221" s="33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B221" s="25">
         <v>287421</v>
@@ -8342,7 +8342,7 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A222" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B222" s="25">
         <v>289219</v>
@@ -8450,7 +8450,7 @@
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A226" s="33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B226" s="27">
         <v>299237</v>
@@ -8540,7 +8540,7 @@
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A229" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B229" s="27">
         <v>306086</v>
@@ -8624,7 +8624,7 @@
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A232" s="33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B232" s="25">
         <v>319381</v>
@@ -8654,7 +8654,7 @@
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A233" s="33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B233" s="25">
         <v>322864</v>
@@ -8684,7 +8684,7 @@
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A234" s="33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B234" s="25">
         <v>325331</v>
@@ -8714,7 +8714,7 @@
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A235" s="33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B235" s="29">
         <v>329453</v>
@@ -8744,7 +8744,7 @@
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A236" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B236" s="29">
         <v>334585</v>
@@ -8772,7 +8772,7 @@
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A237" s="33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B237" s="29">
         <v>341223</v>
@@ -8800,7 +8800,7 @@
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A238" s="33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B238" s="25">
         <v>348557</v>
@@ -8827,7 +8827,7 @@
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A239" s="33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B239" s="27">
         <v>356387</v>
@@ -8857,7 +8857,7 @@
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A240" s="33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B240" s="29">
         <v>361974</v>
@@ -8885,7 +8885,7 @@
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A241" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B241" s="27">
         <v>366299</v>
@@ -8915,7 +8915,7 @@
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A242" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B242" s="27">
         <v>373167</v>
@@ -8945,7 +8945,7 @@
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A243" s="33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B243" s="27">
         <v>380762</v>
@@ -8975,7 +8975,7 @@
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A244" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B244" s="25">
         <v>392049</v>
@@ -9005,7 +9005,7 @@
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A245" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B245" s="25">
         <v>403291</v>
@@ -9035,7 +9035,7 @@
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A246" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B246" s="25">
         <v>418005</v>
@@ -9062,7 +9062,7 @@
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A247" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B247" s="25">
         <v>429181</v>
@@ -9089,7 +9089,7 @@
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A248" s="33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B248" s="25">
         <v>437866</v>
@@ -9170,7 +9170,7 @@
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A251" s="33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B251" s="27">
         <v>481013</v>
@@ -9200,7 +9200,7 @@
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A252" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B252" s="25">
         <v>499694</v>
@@ -9230,7 +9230,7 @@
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A253" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B253" s="25">
         <v>518753</v>
@@ -9260,7 +9260,7 @@
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A254" s="33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B254" s="27">
         <v>532930</v>
@@ -9290,7 +9290,7 @@
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A255" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B255" s="27">
         <v>545027</v>
@@ -9320,7 +9320,7 @@
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A256" s="33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B256" s="27">
         <v>560379</v>
@@ -9350,7 +9350,7 @@
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A257" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B257" s="27">
         <v>577593</v>
@@ -9380,7 +9380,7 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A258" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B258" s="25">
         <v>597583</v>
@@ -9410,7 +9410,7 @@
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A259" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B259" s="25">
         <v>619089</v>
@@ -9440,7 +9440,7 @@
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A260" s="33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B260" s="25">
         <v>642488</v>
@@ -9470,7 +9470,7 @@
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A261" s="33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B261" s="25">
         <v>658505</v>
@@ -9500,7 +9500,7 @@
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A262" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B262" s="27">
         <v>671868</v>
@@ -9530,7 +9530,7 @@
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A263" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B263" s="25">
         <v>687200</v>
@@ -9560,7 +9560,7 @@
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A264" s="33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B264" s="27">
         <v>705687</v>
@@ -9590,7 +9590,7 @@
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A265" s="33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B265" s="25">
         <v>727553</v>
@@ -9620,7 +9620,7 @@
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A266" s="33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B266" s="25">
         <v>751095</v>
@@ -9650,7 +9650,7 @@
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A267" s="33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B267" s="25">
         <v>773556</v>
@@ -9680,7 +9680,7 @@
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A268" s="32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B268" s="25">
         <v>790503</v>
@@ -9710,7 +9710,7 @@
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A269" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B269" s="25">
         <v>801327</v>
@@ -9740,7 +9740,7 @@
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A270" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B270" s="25">
         <v>815746</v>
@@ -9770,7 +9770,7 @@
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A271" s="32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B271" s="25">
         <v>833307</v>
@@ -9830,7 +9830,7 @@
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A273" s="32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B273" s="25">
         <v>879564</v>
@@ -10817,7 +10817,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A2:HB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="GS23" sqref="GS23"/>
     </sheetView>
   </sheetViews>
@@ -10829,7 +10829,7 @@
   <sheetData>
     <row r="2" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:210" x14ac:dyDescent="0.45">
@@ -11463,7 +11463,7 @@
     </row>
     <row r="4" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>908</v>
@@ -12065,7 +12065,7 @@
     </row>
     <row r="5" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>1318</v>
@@ -12667,7 +12667,7 @@
     </row>
     <row r="6" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>276</v>
@@ -13269,7 +13269,7 @@
     </row>
     <row r="7" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3">
         <v>125</v>
@@ -13871,7 +13871,7 @@
     </row>
     <row r="8" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3">
         <v>119</v>
@@ -14473,7 +14473,7 @@
     </row>
     <row r="9" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3">
         <v>95</v>
@@ -15075,7 +15075,7 @@
     </row>
     <row r="10" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3">
         <v>447</v>
@@ -15677,7 +15677,7 @@
     </row>
     <row r="11" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3">
         <v>23</v>
@@ -16279,7 +16279,7 @@
     </row>
     <row r="12" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>361</v>
@@ -16881,7 +16881,7 @@
     </row>
     <row r="13" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3">
         <v>1465</v>
@@ -17483,7 +17483,7 @@
     </row>
     <row r="14" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3">
         <v>208</v>
@@ -18085,7 +18085,7 @@
     </row>
     <row r="15" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3">
         <v>94</v>
@@ -18687,7 +18687,7 @@
     </row>
     <row r="16" spans="1:210" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="3">
         <v>149</v>
@@ -19289,7 +19289,7 @@
     </row>
     <row r="17" spans="1:200" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3">
         <v>54</v>
@@ -19891,7 +19891,7 @@
     </row>
     <row r="18" spans="1:200" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3">
         <v>140</v>
@@ -20493,7 +20493,7 @@
     </row>
     <row r="19" spans="1:200" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3">
         <v>198</v>
@@ -21095,7 +21095,7 @@
     </row>
     <row r="20" spans="1:200" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" s="12">
         <v>5980</v>
@@ -21770,7 +21770,7 @@
   <sheetData>
     <row r="2" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:211" x14ac:dyDescent="0.45">
@@ -22404,10 +22404,10 @@
     </row>
     <row r="4" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="13">
         <v>7.3636366546891958</v>
@@ -23019,10 +23019,10 @@
     </row>
     <row r="5" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="13">
         <v>7.1339550886405885</v>
@@ -23634,10 +23634,10 @@
     </row>
     <row r="6" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="13">
         <v>3.6538082859053489</v>
@@ -24249,10 +24249,10 @@
     </row>
     <row r="7" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="13">
         <v>10.078979279285686</v>
@@ -24864,10 +24864,10 @@
     </row>
     <row r="8" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="13">
         <v>8.1694558155400454</v>
@@ -25479,10 +25479,10 @@
     </row>
     <row r="9" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="13">
         <v>17.423490379012161</v>
@@ -26094,10 +26094,10 @@
     </row>
     <row r="10" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="13">
         <v>8.2026947297596031</v>
@@ -26709,10 +26709,10 @@
     </row>
     <row r="11" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="13">
         <v>5.0919937211800503</v>
@@ -27324,10 +27324,10 @@
     </row>
     <row r="12" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="13">
         <v>9.4900702568073587</v>
@@ -27939,10 +27939,10 @@
     </row>
     <row r="13" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="13">
         <v>5.1597373204886656</v>
@@ -28554,10 +28554,10 @@
     </row>
     <row r="14" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A14" s="34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="13">
         <v>9.2387589267175123</v>
@@ -29169,10 +29169,10 @@
     </row>
     <row r="15" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="13">
         <v>4.5224221942942817</v>
@@ -29784,10 +29784,10 @@
     </row>
     <row r="16" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16" s="13">
         <v>4.9762790729152275</v>
@@ -30399,10 +30399,10 @@
     </row>
     <row r="17" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="13">
         <v>2.4452966756191694</v>
@@ -31014,10 +31014,10 @@
     </row>
     <row r="18" spans="1:211" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="13">
         <v>4.8330659036866628</v>
@@ -31629,10 +31629,10 @@
     </row>
     <row r="19" spans="1:211" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19" s="13">
         <v>1.4288598630158262</v>
@@ -32244,10 +32244,10 @@
     </row>
     <row r="20" spans="1:211" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="15">
         <v>7.1941983001360574</v>
@@ -32881,7 +32881,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" s="16"/>
     </row>
@@ -32893,18 +32893,18 @@
     </row>
     <row r="5" spans="1:3" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>103</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B6">
         <v>181</v>
@@ -32915,7 +32915,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7">
         <v>964</v>
@@ -32926,7 +32926,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B8">
         <v>503</v>
@@ -32937,7 +32937,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9">
         <v>410</v>
@@ -32948,7 +32948,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10">
         <v>765</v>
@@ -32959,7 +32959,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B11">
         <v>994</v>
@@ -32970,7 +32970,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B12">
         <v>242</v>
@@ -32981,7 +32981,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13">
         <v>137</v>
@@ -32992,7 +32992,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14">
         <v>191</v>
@@ -33003,7 +33003,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15">
         <v>847</v>
@@ -33014,7 +33014,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16">
         <v>318</v>
@@ -33025,7 +33025,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17">
         <v>501</v>
@@ -33036,7 +33036,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B18">
         <v>1060</v>
@@ -33047,7 +33047,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19">
         <v>968</v>
@@ -33058,7 +33058,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B20">
         <v>1339</v>
@@ -33069,7 +33069,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B21">
         <v>420</v>
@@ -33080,7 +33080,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B22">
         <v>870</v>
@@ -33091,7 +33091,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B23">
         <v>258</v>
@@ -33102,7 +33102,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B24">
         <v>661</v>
@@ -33113,7 +33113,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B25">
         <v>469</v>
@@ -33124,7 +33124,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B26">
         <v>644</v>
@@ -33135,7 +33135,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B27">
         <v>474</v>
@@ -33146,7 +33146,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B28">
         <v>310</v>
@@ -33157,7 +33157,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B29">
         <v>828</v>
@@ -33168,7 +33168,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B30">
         <v>300</v>
@@ -33179,7 +33179,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B31">
         <v>158</v>
@@ -33190,7 +33190,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B32">
         <v>119</v>
@@ -33201,7 +33201,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B33">
         <v>336</v>
@@ -33212,7 +33212,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B34">
         <v>608</v>
@@ -33223,7 +33223,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B35">
         <v>726</v>
@@ -33234,7 +33234,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B36">
         <v>326</v>
@@ -33245,7 +33245,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B37">
         <v>270</v>
@@ -33256,7 +33256,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B38">
         <v>524</v>
@@ -33267,7 +33267,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B39">
         <v>947</v>
@@ -33278,7 +33278,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B40">
         <v>265</v>
@@ -33289,7 +33289,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B41">
         <v>679</v>
@@ -33300,7 +33300,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B42">
         <v>1153</v>
@@ -33311,7 +33311,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B43">
         <v>577</v>
@@ -33322,7 +33322,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B44">
         <v>758</v>
@@ -33333,7 +33333,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B45">
         <v>412</v>
@@ -33344,7 +33344,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B46">
         <v>232</v>
@@ -33355,7 +33355,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B47">
         <v>477</v>
@@ -33366,7 +33366,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B48">
         <v>1278</v>
@@ -33377,7 +33377,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B49">
         <v>546</v>
@@ -33388,7 +33388,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B50">
         <v>1643</v>
@@ -33399,7 +33399,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B51">
         <v>166</v>
@@ -33410,7 +33410,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B52">
         <v>136</v>
@@ -33421,7 +33421,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B53">
         <v>266</v>
@@ -33432,7 +33432,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B54">
         <v>575</v>
@@ -33443,7 +33443,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B55">
         <v>630</v>
@@ -33454,7 +33454,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B56">
         <v>286</v>
@@ -33465,7 +33465,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B57">
         <v>741</v>
@@ -33476,7 +33476,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B58">
         <v>517</v>
@@ -33487,7 +33487,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B59">
         <v>256</v>
@@ -33498,7 +33498,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B60">
         <v>638</v>
@@ -33509,7 +33509,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B61">
         <v>201</v>
@@ -33520,7 +33520,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B62">
         <v>514</v>
@@ -33531,7 +33531,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B63">
         <v>347</v>
@@ -33542,7 +33542,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B64">
         <v>253</v>
@@ -33553,7 +33553,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B65">
         <v>550</v>
@@ -33564,7 +33564,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B66">
         <v>705</v>
@@ -33575,7 +33575,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B67">
         <v>140</v>
@@ -33586,7 +33586,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B68">
         <v>343</v>
@@ -33597,7 +33597,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B69">
         <v>325</v>
@@ -33608,7 +33608,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B70">
         <v>496</v>
@@ -33619,7 +33619,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B71">
         <v>244</v>
@@ -33630,7 +33630,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B72">
         <v>366</v>
@@ -33641,7 +33641,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B73">
         <v>189</v>
@@ -33652,7 +33652,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B74">
         <v>319</v>
@@ -33663,7 +33663,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B75">
         <v>1146</v>
@@ -33674,7 +33674,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B76">
         <v>131</v>
@@ -33685,7 +33685,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B77">
         <v>460</v>
@@ -33696,7 +33696,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B78">
         <v>191</v>
@@ -33707,7 +33707,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B79">
         <v>615</v>
@@ -33718,7 +33718,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B80">
         <v>316</v>
@@ -33729,7 +33729,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B81">
         <v>569</v>
@@ -33740,7 +33740,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B82">
         <v>77</v>
@@ -33751,7 +33751,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B83">
         <v>203</v>
@@ -33762,7 +33762,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B84">
         <v>858</v>
@@ -33773,7 +33773,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B85">
         <v>875</v>
@@ -33784,7 +33784,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B86">
         <v>239</v>
@@ -33795,7 +33795,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B87">
         <v>230</v>
@@ -33806,7 +33806,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B88">
         <v>206</v>
@@ -33817,7 +33817,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B89">
         <v>236</v>
@@ -33828,7 +33828,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B90">
         <v>281</v>
@@ -33839,7 +33839,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B91">
         <v>628</v>
@@ -33850,7 +33850,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B92">
         <v>370</v>
@@ -33861,7 +33861,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B93">
         <v>280</v>
@@ -33872,7 +33872,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B94">
         <v>414</v>
@@ -33883,7 +33883,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B95">
         <v>971</v>
@@ -33894,7 +33894,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B96">
         <v>185</v>
@@ -33905,7 +33905,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B97">
         <v>131</v>
@@ -33916,7 +33916,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B98">
         <v>271</v>
@@ -33927,7 +33927,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B99">
         <v>100</v>
@@ -33938,7 +33938,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B100">
         <v>268</v>
@@ -33949,7 +33949,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B101">
         <v>468</v>
@@ -33960,7 +33960,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B102">
         <v>410</v>
@@ -33971,7 +33971,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B103">
         <v>245</v>
@@ -33982,7 +33982,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B104">
         <v>619</v>
@@ -33993,7 +33993,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B105">
         <v>259</v>
@@ -34004,7 +34004,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B106">
         <v>290</v>
@@ -34015,7 +34015,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B107">
         <v>77</v>
@@ -34026,7 +34026,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B108">
         <v>2488</v>
@@ -34037,7 +34037,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B109">
         <v>230</v>
@@ -34048,7 +34048,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B110">
         <v>399</v>
@@ -34059,7 +34059,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B111">
         <v>223</v>
@@ -34070,7 +34070,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B112">
         <v>71</v>
@@ -34081,7 +34081,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B113">
         <v>171</v>
@@ -34092,7 +34092,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B114">
         <v>244</v>
@@ -34103,7 +34103,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B115">
         <v>200</v>
@@ -34114,7 +34114,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B116">
         <v>190</v>
@@ -34125,7 +34125,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B117">
         <v>443</v>
@@ -34136,7 +34136,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B118">
         <v>113</v>
@@ -34147,7 +34147,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B119">
         <v>167</v>
@@ -34158,7 +34158,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B120">
         <v>894</v>
@@ -34169,7 +34169,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B121">
         <v>451</v>
@@ -34180,7 +34180,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B122">
         <v>544</v>
@@ -34191,7 +34191,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B123">
         <v>205</v>
@@ -34202,7 +34202,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B124">
         <v>398</v>
@@ -34213,7 +34213,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B125">
         <v>1001</v>
@@ -34224,7 +34224,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B126">
         <v>130</v>
@@ -34235,7 +34235,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B127">
         <v>911</v>
@@ -34246,7 +34246,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B128">
         <v>320</v>
@@ -34257,7 +34257,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B129">
         <v>445</v>
@@ -34268,7 +34268,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B130">
         <v>362</v>
@@ -34279,7 +34279,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B131">
         <v>207</v>
@@ -34290,7 +34290,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B132">
         <v>1730</v>
@@ -34301,7 +34301,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B133">
         <v>206</v>
@@ -34312,7 +34312,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B134">
         <v>65</v>
@@ -34323,7 +34323,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B135">
         <v>488</v>
@@ -34334,7 +34334,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B136">
         <v>213</v>
@@ -34345,7 +34345,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B137">
         <v>158</v>
@@ -34356,7 +34356,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B138">
         <v>202</v>
@@ -34367,7 +34367,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B139">
         <v>673</v>
@@ -34378,7 +34378,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B140">
         <v>345</v>
@@ -34389,7 +34389,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B141">
         <v>114</v>
@@ -34400,7 +34400,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B142">
         <v>407</v>
@@ -34411,7 +34411,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B143">
         <v>151</v>
@@ -34422,7 +34422,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B144">
         <v>128</v>
@@ -34433,7 +34433,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B145">
         <v>466</v>
@@ -34444,7 +34444,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B146">
         <v>579</v>
@@ -34455,7 +34455,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B147">
         <v>546</v>
@@ -34466,7 +34466,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B148">
         <v>199</v>
@@ -34477,7 +34477,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B149">
         <v>150</v>
@@ -34488,7 +34488,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B150">
         <v>213</v>
@@ -34499,7 +34499,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B151">
         <v>174</v>
@@ -34510,7 +34510,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B152">
         <v>508</v>
@@ -34521,7 +34521,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B153">
         <v>302</v>
@@ -34532,7 +34532,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B154">
         <v>478</v>
@@ -34543,7 +34543,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B155">
         <v>158</v>
@@ -34554,7 +34554,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B156">
         <v>242</v>
@@ -34565,7 +34565,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B157">
         <v>146</v>
@@ -34576,7 +34576,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B158">
         <v>219</v>
@@ -34587,7 +34587,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B159">
         <v>377</v>
@@ -34598,7 +34598,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B160">
         <v>692</v>
@@ -34609,7 +34609,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B161">
         <v>92</v>
@@ -34620,7 +34620,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B162">
         <v>614</v>
@@ -34631,7 +34631,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B163">
         <v>126</v>
@@ -34642,7 +34642,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B164">
         <v>594</v>
@@ -34653,7 +34653,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B165">
         <v>330</v>
@@ -34664,7 +34664,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B166">
         <v>314</v>
@@ -34675,7 +34675,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B167">
         <v>161</v>
@@ -34686,7 +34686,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B168">
         <v>633</v>
@@ -34697,7 +34697,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B169">
         <v>437</v>
@@ -34708,7 +34708,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B170">
         <v>854</v>
@@ -34719,7 +34719,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B171">
         <v>78</v>
@@ -34730,7 +34730,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B172">
         <v>179</v>
@@ -34741,7 +34741,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B173">
         <v>205</v>
@@ -34752,7 +34752,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B174">
         <v>183</v>
@@ -34763,7 +34763,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B175">
         <v>124</v>
@@ -34774,7 +34774,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B176">
         <v>409</v>
@@ -34785,7 +34785,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B177">
         <v>180</v>
@@ -34796,7 +34796,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B178">
         <v>907</v>
@@ -34807,7 +34807,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B179">
         <v>404</v>
@@ -34818,7 +34818,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B180">
         <v>243</v>
@@ -34829,7 +34829,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B181">
         <v>847</v>
@@ -34840,7 +34840,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B182">
         <v>404</v>
@@ -34851,7 +34851,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B183">
         <v>245</v>
@@ -34862,7 +34862,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B184">
         <v>305</v>
@@ -34873,7 +34873,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B185">
         <v>750</v>
@@ -34884,7 +34884,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B186">
         <v>228</v>
@@ -34895,7 +34895,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B187">
         <v>132</v>
@@ -34906,7 +34906,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B188">
         <v>139</v>
@@ -34917,7 +34917,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B189">
         <v>100</v>
@@ -34928,7 +34928,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B190">
         <v>84</v>
@@ -34939,7 +34939,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B191">
         <v>124</v>
@@ -34950,7 +34950,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B192">
         <v>61</v>
@@ -34961,7 +34961,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B193">
         <v>385</v>
@@ -34972,7 +34972,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B194">
         <v>621</v>
@@ -34983,7 +34983,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B195">
         <v>252</v>
@@ -34994,7 +34994,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B196">
         <v>233</v>
@@ -35005,7 +35005,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B197">
         <v>263</v>
@@ -35016,7 +35016,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B198">
         <v>66</v>
@@ -35027,7 +35027,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B199">
         <v>100</v>
@@ -35038,7 +35038,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B200">
         <v>385</v>
@@ -35049,7 +35049,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B201">
         <v>531</v>
@@ -35060,7 +35060,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B202">
         <v>178</v>
@@ -35071,7 +35071,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B203">
         <v>239</v>
@@ -35082,7 +35082,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B204">
         <v>340</v>
@@ -35093,7 +35093,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B205">
         <v>110</v>
@@ -35104,7 +35104,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B206">
         <v>346</v>
@@ -35115,7 +35115,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B207">
         <v>432</v>
@@ -35126,7 +35126,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B208">
         <v>332</v>
@@ -35137,7 +35137,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B209">
         <v>254</v>
@@ -35148,7 +35148,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B210">
         <v>202</v>
@@ -35159,7 +35159,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B211">
         <v>115</v>
@@ -35170,7 +35170,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B212">
         <v>116</v>
@@ -35181,7 +35181,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B213">
         <v>237</v>
@@ -35192,7 +35192,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B214">
         <v>209</v>
@@ -35203,7 +35203,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B215">
         <v>703</v>
@@ -35214,7 +35214,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B216">
         <v>342</v>
@@ -35225,7 +35225,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B217">
         <v>503</v>
@@ -35236,7 +35236,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B218">
         <v>85</v>
@@ -35247,7 +35247,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B219">
         <v>172</v>
@@ -35258,7 +35258,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B220">
         <v>118</v>
@@ -35269,7 +35269,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B221">
         <v>263</v>
@@ -35280,7 +35280,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B222">
         <v>51</v>
@@ -35291,7 +35291,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B223">
         <v>103</v>
@@ -35302,7 +35302,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B224">
         <v>194</v>
@@ -35313,7 +35313,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B225">
         <v>88</v>
@@ -35324,7 +35324,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B226">
         <v>244</v>
@@ -35335,7 +35335,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B227">
         <v>139</v>
@@ -35346,7 +35346,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B228">
         <v>97</v>
@@ -35357,7 +35357,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B229">
         <v>259</v>
@@ -35368,7 +35368,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B230">
         <v>670</v>
@@ -35379,7 +35379,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B231">
         <v>390</v>
@@ -35390,7 +35390,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B232">
         <v>127</v>
@@ -35401,7 +35401,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B233">
         <v>190</v>
@@ -35412,7 +35412,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B234">
         <v>532</v>
@@ -35423,7 +35423,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B235">
         <v>137</v>
@@ -35434,7 +35434,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B236">
         <v>304</v>
@@ -35445,7 +35445,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B237">
         <v>91</v>
@@ -35456,7 +35456,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B238">
         <v>131</v>
@@ -35467,7 +35467,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B239">
         <v>139</v>
@@ -35478,7 +35478,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B240">
         <v>400</v>
@@ -35489,7 +35489,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B241">
         <v>157</v>
@@ -35500,7 +35500,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B242">
         <v>139</v>
@@ -35511,7 +35511,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B243">
         <v>155</v>
@@ -35522,7 +35522,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B244">
         <v>351</v>
@@ -35533,7 +35533,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B245">
         <v>134</v>
@@ -35544,7 +35544,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B246">
         <v>110</v>
@@ -35555,7 +35555,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B247">
         <v>166</v>
@@ -35566,7 +35566,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B248">
         <v>128</v>
@@ -35577,7 +35577,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B249">
         <v>166</v>
@@ -35588,7 +35588,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B250">
         <v>156</v>
@@ -35599,7 +35599,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B251">
         <v>147</v>
@@ -35610,7 +35610,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B252">
         <v>182</v>
@@ -35621,7 +35621,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B253">
         <v>63</v>
@@ -35632,7 +35632,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B254">
         <v>103</v>
@@ -35643,7 +35643,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B255">
         <v>292</v>
@@ -35654,7 +35654,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B256">
         <v>148</v>
@@ -35665,7 +35665,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B257">
         <v>90</v>
@@ -35676,7 +35676,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B258">
         <v>153</v>
@@ -35687,7 +35687,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B259">
         <v>254</v>
@@ -35698,7 +35698,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B260">
         <v>106</v>
@@ -35709,7 +35709,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B261">
         <v>59</v>
@@ -35720,7 +35720,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B262">
         <v>469</v>
@@ -35731,7 +35731,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B263">
         <v>199</v>
@@ -35742,7 +35742,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B264">
         <v>326</v>
@@ -35753,7 +35753,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B265">
         <v>72</v>
@@ -35764,7 +35764,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B266">
         <v>208</v>
@@ -35775,7 +35775,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B267">
         <v>94</v>
@@ -35786,7 +35786,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B268">
         <v>1873</v>
@@ -35797,7 +35797,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B269">
         <v>126</v>
@@ -35808,7 +35808,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B270">
         <v>314</v>
@@ -35819,7 +35819,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B271">
         <v>144</v>
@@ -35830,7 +35830,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B272">
         <v>137</v>
@@ -35841,7 +35841,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B273">
         <v>131</v>
@@ -35852,7 +35852,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B274">
         <v>184</v>
@@ -35863,7 +35863,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B275">
         <v>229</v>
@@ -35874,7 +35874,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B276">
         <v>111</v>
@@ -35885,7 +35885,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B277">
         <v>93</v>
@@ -35896,7 +35896,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B278">
         <v>101</v>
@@ -35907,7 +35907,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B279">
         <v>137</v>
@@ -35918,7 +35918,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B280">
         <v>131</v>
@@ -35929,7 +35929,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B281">
         <v>174</v>
@@ -35940,7 +35940,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B282">
         <v>84</v>
@@ -35951,7 +35951,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B283">
         <v>46</v>
@@ -35962,7 +35962,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B284">
         <v>123</v>
@@ -35973,7 +35973,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B285">
         <v>45</v>
@@ -35984,7 +35984,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B286">
         <v>208</v>
@@ -35995,7 +35995,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B287">
         <v>204</v>
@@ -36006,7 +36006,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B288">
         <v>97</v>
@@ -36017,7 +36017,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B289">
         <v>309</v>
@@ -36028,7 +36028,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B290">
         <v>216</v>
@@ -36039,7 +36039,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B291">
         <v>107</v>
@@ -36050,7 +36050,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B292">
         <v>182</v>
@@ -36061,7 +36061,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B293">
         <v>158</v>
@@ -36072,7 +36072,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B294">
         <v>150</v>
@@ -36083,7 +36083,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B295">
         <v>31</v>
@@ -36094,7 +36094,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B296">
         <v>82</v>
@@ -36105,7 +36105,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B297">
         <v>146</v>
@@ -36116,7 +36116,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B298">
         <v>72</v>
@@ -36127,7 +36127,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B299">
         <v>94</v>
@@ -36138,7 +36138,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B300">
         <v>101</v>
@@ -36149,7 +36149,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B301">
         <v>253</v>
@@ -36160,7 +36160,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B302">
         <v>159</v>
@@ -36171,7 +36171,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B303">
         <v>116</v>
@@ -36182,7 +36182,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B304">
         <v>122</v>
@@ -36193,7 +36193,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B305">
         <v>104</v>
@@ -36204,7 +36204,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B306">
         <v>227</v>
@@ -36215,7 +36215,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B307">
         <v>95</v>
@@ -36226,7 +36226,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B308">
         <v>135</v>
@@ -36237,7 +36237,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B309">
         <v>197</v>
@@ -36248,7 +36248,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B310">
         <v>171</v>
@@ -36259,7 +36259,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B311">
         <v>35</v>
@@ -36270,7 +36270,7 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B312">
         <v>202</v>
@@ -36281,7 +36281,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B313">
         <v>76</v>
@@ -36292,7 +36292,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B314">
         <v>956</v>
@@ -36303,7 +36303,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B315">
         <v>80</v>
@@ -36314,7 +36314,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B316">
         <v>184</v>
@@ -36325,7 +36325,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B317">
         <v>109</v>
@@ -36336,7 +36336,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B318">
         <v>127</v>
@@ -36347,7 +36347,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B319">
         <v>105</v>
@@ -36358,7 +36358,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B320">
         <v>136</v>
@@ -36369,7 +36369,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B321">
         <v>96</v>
@@ -36380,7 +36380,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B322">
         <v>78</v>
@@ -36391,7 +36391,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B323">
         <v>41</v>
@@ -36402,7 +36402,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B324">
         <v>242</v>
@@ -36413,7 +36413,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B325">
         <v>137</v>
@@ -36424,7 +36424,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B326">
         <v>85</v>
@@ -36435,7 +36435,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B327">
         <v>59</v>
@@ -36446,7 +36446,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B328">
         <v>239</v>
@@ -36457,7 +36457,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B329">
         <v>135</v>
@@ -36468,7 +36468,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B330">
         <v>135</v>
@@ -36479,7 +36479,7 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B331">
         <v>77</v>
@@ -36490,7 +36490,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B332">
         <v>77</v>
@@ -36501,7 +36501,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B333">
         <v>175</v>
@@ -36512,7 +36512,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B334">
         <v>90</v>
@@ -36523,7 +36523,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B335">
         <v>154</v>
@@ -36534,7 +36534,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B336">
         <v>429</v>
@@ -36545,7 +36545,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B337">
         <v>36</v>
@@ -36556,7 +36556,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B338">
         <v>176</v>
@@ -36567,7 +36567,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B339">
         <v>72</v>
@@ -36578,7 +36578,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B340">
         <v>157</v>
@@ -36589,7 +36589,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B341">
         <v>93</v>
@@ -36600,7 +36600,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B342">
         <v>114</v>
@@ -36611,7 +36611,7 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B343">
         <v>190</v>
@@ -36622,7 +36622,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B344">
         <v>163</v>
@@ -36633,7 +36633,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B345">
         <v>55</v>
@@ -36644,7 +36644,7 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B346">
         <v>27</v>
@@ -36655,7 +36655,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B347">
         <v>86</v>
@@ -36666,7 +36666,7 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B348">
         <v>83</v>
@@ -36677,7 +36677,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B349">
         <v>83</v>
@@ -36688,7 +36688,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B350">
         <v>122</v>
@@ -36699,7 +36699,7 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B351">
         <v>182</v>
@@ -36710,7 +36710,7 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B352">
         <v>106</v>
@@ -36721,7 +36721,7 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B353">
         <v>54</v>
@@ -36732,7 +36732,7 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B354">
         <v>96</v>
@@ -36743,7 +36743,7 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B355">
         <v>125</v>
@@ -36754,7 +36754,7 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B356">
         <v>99</v>
@@ -36765,7 +36765,7 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B357">
         <v>77</v>
@@ -36776,7 +36776,7 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B358">
         <v>63</v>
@@ -36787,7 +36787,7 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B359">
         <v>44</v>
@@ -36798,7 +36798,7 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B360">
         <v>182</v>
@@ -36809,7 +36809,7 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B361">
         <v>72</v>
@@ -36820,7 +36820,7 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B362">
         <v>130</v>
@@ -36831,7 +36831,7 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B363">
         <v>118</v>
@@ -36842,7 +36842,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B364">
         <v>112</v>
@@ -36853,7 +36853,7 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B365">
         <v>48</v>
@@ -36864,7 +36864,7 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B366">
         <v>188</v>
@@ -36875,7 +36875,7 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B367">
         <v>97</v>
@@ -36886,7 +36886,7 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B368">
         <v>108</v>
@@ -36897,7 +36897,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B369">
         <v>63</v>
@@ -36908,7 +36908,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B370">
         <v>52</v>
@@ -36919,7 +36919,7 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B371">
         <v>111</v>
@@ -36930,7 +36930,7 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B372">
         <v>128</v>
@@ -36941,7 +36941,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B373">
         <v>131</v>
@@ -36952,7 +36952,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B374">
         <v>135</v>
@@ -36963,7 +36963,7 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B375">
         <v>70</v>
@@ -36974,7 +36974,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B376">
         <v>109</v>
@@ -36985,7 +36985,7 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B377">
         <v>90</v>
@@ -36996,7 +36996,7 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B378">
         <v>45</v>
@@ -37007,7 +37007,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B379">
         <v>48</v>
@@ -37018,7 +37018,7 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B380">
         <v>31</v>
@@ -37029,7 +37029,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B381">
         <v>23</v>
@@ -37040,7 +37040,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B382">
         <v>94</v>
@@ -37051,7 +37051,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B383">
         <v>78</v>
@@ -37062,7 +37062,7 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B384">
         <v>17</v>
@@ -37073,7 +37073,7 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B385">
         <v>32</v>
@@ -37084,7 +37084,7 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B386">
         <v>94</v>
@@ -37095,7 +37095,7 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B387">
         <v>33</v>
@@ -37106,7 +37106,7 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B388">
         <v>75</v>
@@ -37117,7 +37117,7 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B389">
         <v>52</v>
@@ -37128,7 +37128,7 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B390">
         <v>108</v>
@@ -37139,7 +37139,7 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B391">
         <v>57</v>
@@ -37150,7 +37150,7 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B392">
         <v>42</v>
@@ -37161,7 +37161,7 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B393">
         <v>85</v>
@@ -37172,7 +37172,7 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B394">
         <v>78</v>
@@ -37183,7 +37183,7 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B395">
         <v>90</v>
@@ -37194,7 +37194,7 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B396">
         <v>96</v>
@@ -37205,7 +37205,7 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B397">
         <v>74</v>
@@ -37216,7 +37216,7 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B398">
         <v>48</v>
@@ -37227,7 +37227,7 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B399">
         <v>34</v>
@@ -37238,7 +37238,7 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B400">
         <v>25</v>
@@ -37249,7 +37249,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B401">
         <v>42</v>
@@ -37260,7 +37260,7 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B402">
         <v>75</v>
@@ -37271,7 +37271,7 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B403">
         <v>14</v>
@@ -37282,7 +37282,7 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B404">
         <v>69</v>
@@ -37293,7 +37293,7 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B405">
         <v>55</v>
@@ -37304,7 +37304,7 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B406">
         <v>33</v>
@@ -37315,7 +37315,7 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B407">
         <v>38</v>
@@ -37326,7 +37326,7 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B408">
         <v>24</v>
@@ -37337,7 +37337,7 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B409">
         <v>20</v>
@@ -37348,7 +37348,7 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B410">
         <v>20</v>
@@ -37359,7 +37359,7 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B411">
         <v>21</v>
@@ -37370,7 +37370,7 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B412">
         <v>56</v>
@@ -37381,7 +37381,7 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B413">
         <v>14</v>
@@ -37392,7 +37392,7 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B414">
         <v>67</v>
@@ -37403,7 +37403,7 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B415">
         <v>30</v>
@@ -37414,7 +37414,7 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B416">
         <v>20</v>
@@ -37425,7 +37425,7 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B417">
         <v>26</v>

</xml_diff>